<commit_message>
Correction to time for Jake Rogers.
</commit_message>
<xml_diff>
--- a/2022/com-20220522.xlsx
+++ b/2022/com-20220522.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jrye/personal/mac/results/2022/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{375B929F-A491-494E-B911-C826B8D9CAFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D9CA460-E0D0-AD4E-B2AA-F5AAD60CB178}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="22500" yWindow="500" windowWidth="12700" windowHeight="17140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -430,9 +430,6 @@
     <t xml:space="preserve"> 0:46.066 </t>
   </si>
   <si>
-    <t xml:space="preserve"> 0:46.145 </t>
-  </si>
-  <si>
     <t xml:space="preserve"> 0:49.164</t>
   </si>
   <si>
@@ -440,6 +437,9 @@
   </si>
   <si>
     <t>XB</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0:46.701 </t>
   </si>
 </sst>
 </file>
@@ -1311,8 +1311,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A44" workbookViewId="0">
-      <selection activeCell="B71" sqref="B71"/>
+    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
+      <selection activeCell="E79" sqref="E79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1891,7 +1891,7 @@
     </row>
     <row r="64" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B64" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C64" t="s">
         <v>63</v>
@@ -1964,7 +1964,7 @@
         <v>124</v>
       </c>
       <c r="B70" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C70" t="s">
         <v>68</v>
@@ -2054,7 +2054,7 @@
         <v>75</v>
       </c>
       <c r="E78" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.2">
@@ -2068,7 +2068,7 @@
         <v>77</v>
       </c>
       <c r="E79" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add CVSCC results. Fix some spelling errors in COM results.
</commit_message>
<xml_diff>
--- a/2022/com-20220522.xlsx
+++ b/2022/com-20220522.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10520"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10911"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jrye/personal/mac/results/2022/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{032C7DED-C94E-CD46-B3BD-CE26C0F8CEEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87547205-0BFE-3C4F-815F-7C7A73AB5085}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="22500" yWindow="500" windowWidth="12700" windowHeight="17140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -115,9 +115,6 @@
     <t xml:space="preserve"> STU</t>
   </si>
   <si>
-    <t xml:space="preserve"> MICHAEL HARTL</t>
-  </si>
-  <si>
     <t xml:space="preserve"> STH</t>
   </si>
   <si>
@@ -440,6 +437,9 @@
   </si>
   <si>
     <t xml:space="preserve"> TYLER SALMINEN</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> MIKE HARTL</t>
   </si>
 </sst>
 </file>
@@ -1311,8 +1311,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
-      <selection activeCell="C66" sqref="C66"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1327,19 +1327,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>89</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -1350,7 +1350,7 @@
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E2" t="s">
         <v>2</v>
@@ -1364,7 +1364,7 @@
         <v>3</v>
       </c>
       <c r="D3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E3" t="s">
         <v>2</v>
@@ -1378,7 +1378,7 @@
         <v>5</v>
       </c>
       <c r="D5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E5" t="s">
         <v>2</v>
@@ -1392,7 +1392,7 @@
         <v>6</v>
       </c>
       <c r="D6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E6" t="s">
         <v>2</v>
@@ -1406,7 +1406,7 @@
         <v>7</v>
       </c>
       <c r="D7" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E7" t="s">
         <v>2</v>
@@ -1420,7 +1420,7 @@
         <v>8</v>
       </c>
       <c r="D8" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E8" t="s">
         <v>2</v>
@@ -1434,7 +1434,7 @@
         <v>9</v>
       </c>
       <c r="D9" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E9" t="s">
         <v>2</v>
@@ -1448,7 +1448,7 @@
         <v>10</v>
       </c>
       <c r="D10" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E10" t="s">
         <v>2</v>
@@ -1462,7 +1462,7 @@
         <v>11</v>
       </c>
       <c r="D11" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E11" t="s">
         <v>2</v>
@@ -1476,7 +1476,7 @@
         <v>13</v>
       </c>
       <c r="D13" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E13" t="s">
         <v>2</v>
@@ -1490,7 +1490,7 @@
         <v>14</v>
       </c>
       <c r="D14" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E14" t="s">
         <v>2</v>
@@ -1504,7 +1504,7 @@
         <v>15</v>
       </c>
       <c r="D15" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E15" t="s">
         <v>2</v>
@@ -1518,7 +1518,7 @@
         <v>17</v>
       </c>
       <c r="D17" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E17" t="s">
         <v>2</v>
@@ -1532,7 +1532,7 @@
         <v>19</v>
       </c>
       <c r="D19" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E19" t="s">
         <v>2</v>
@@ -1546,7 +1546,7 @@
         <v>20</v>
       </c>
       <c r="D20" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E20" t="s">
         <v>2</v>
@@ -1560,7 +1560,7 @@
         <v>21</v>
       </c>
       <c r="D21" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E21" t="s">
         <v>2</v>
@@ -1574,7 +1574,7 @@
         <v>23</v>
       </c>
       <c r="D23" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E23" t="s">
         <v>2</v>
@@ -1588,7 +1588,7 @@
         <v>25</v>
       </c>
       <c r="D25" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E25" t="s">
         <v>2</v>
@@ -1602,7 +1602,7 @@
         <v>27</v>
       </c>
       <c r="D27" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E27" t="s">
         <v>2</v>
@@ -1616,7 +1616,7 @@
         <v>29</v>
       </c>
       <c r="D29" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E29" t="s">
         <v>2</v>
@@ -1627,109 +1627,109 @@
         <v>30</v>
       </c>
       <c r="C31" t="s">
-        <v>31</v>
+        <v>139</v>
       </c>
       <c r="D31" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="33" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B33" t="s">
+        <v>31</v>
+      </c>
+      <c r="C33" t="s">
         <v>32</v>
       </c>
-      <c r="C33" t="s">
-        <v>33</v>
-      </c>
       <c r="D33" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="35" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B35" t="s">
+        <v>33</v>
+      </c>
+      <c r="C35" t="s">
         <v>34</v>
       </c>
-      <c r="C35" t="s">
-        <v>35</v>
-      </c>
       <c r="D35" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="37" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B37" t="s">
+        <v>35</v>
+      </c>
+      <c r="C37" t="s">
         <v>36</v>
       </c>
-      <c r="C37" t="s">
-        <v>37</v>
-      </c>
       <c r="D37" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="39" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B39" t="s">
+        <v>37</v>
+      </c>
+      <c r="C39" t="s">
         <v>38</v>
       </c>
-      <c r="C39" t="s">
-        <v>39</v>
-      </c>
       <c r="D39" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="41" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B41" t="s">
+        <v>39</v>
+      </c>
+      <c r="C41" t="s">
         <v>40</v>
       </c>
-      <c r="C41" t="s">
-        <v>41</v>
-      </c>
       <c r="D41" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="43" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B43" t="s">
+        <v>41</v>
+      </c>
+      <c r="C43" t="s">
         <v>42</v>
       </c>
-      <c r="C43" t="s">
-        <v>43</v>
-      </c>
       <c r="D43" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="44" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B44" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C44" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D44" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="45" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B45" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C45" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D45" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="47" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B47" t="s">
+        <v>45</v>
+      </c>
+      <c r="C47" t="s">
         <v>46</v>
       </c>
-      <c r="C47" t="s">
-        <v>47</v>
-      </c>
       <c r="D47" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E47" t="s">
         <v>2</v>
@@ -1737,13 +1737,13 @@
     </row>
     <row r="48" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B48" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C48" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D48" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E48" t="s">
         <v>2</v>
@@ -1751,13 +1751,13 @@
     </row>
     <row r="49" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B49" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C49" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D49" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E49" t="s">
         <v>2</v>
@@ -1765,13 +1765,13 @@
     </row>
     <row r="50" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B50" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C50" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D50" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E50" t="s">
         <v>2</v>
@@ -1779,13 +1779,13 @@
     </row>
     <row r="52" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B52" t="s">
+        <v>50</v>
+      </c>
+      <c r="C52" t="s">
         <v>51</v>
       </c>
-      <c r="C52" t="s">
-        <v>52</v>
-      </c>
       <c r="D52" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E52" t="s">
         <v>2</v>
@@ -1793,13 +1793,13 @@
     </row>
     <row r="53" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B53" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C53" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D53" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E53" t="s">
         <v>2</v>
@@ -1807,13 +1807,13 @@
     </row>
     <row r="54" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B54" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C54" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D54" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E54" t="s">
         <v>2</v>
@@ -1821,13 +1821,13 @@
     </row>
     <row r="56" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B56" t="s">
+        <v>54</v>
+      </c>
+      <c r="C56" t="s">
         <v>55</v>
       </c>
-      <c r="C56" t="s">
-        <v>56</v>
-      </c>
       <c r="D56" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E56" t="s">
         <v>2</v>
@@ -1835,13 +1835,13 @@
     </row>
     <row r="57" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B57" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C57" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D57" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E57" t="s">
         <v>2</v>
@@ -1849,13 +1849,13 @@
     </row>
     <row r="59" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B59" t="s">
+        <v>57</v>
+      </c>
+      <c r="C59" t="s">
         <v>58</v>
       </c>
-      <c r="C59" t="s">
-        <v>59</v>
-      </c>
       <c r="D59" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E59" t="s">
         <v>2</v>
@@ -1863,13 +1863,13 @@
     </row>
     <row r="60" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B60" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C60" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D60" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E60" t="s">
         <v>2</v>
@@ -1877,13 +1877,13 @@
     </row>
     <row r="62" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B62" t="s">
+        <v>60</v>
+      </c>
+      <c r="C62" t="s">
         <v>61</v>
       </c>
-      <c r="C62" t="s">
-        <v>62</v>
-      </c>
       <c r="D62" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E62" t="s">
         <v>2</v>
@@ -1891,13 +1891,13 @@
     </row>
     <row r="64" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B64" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C64" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D64" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E64" t="s">
         <v>2</v>
@@ -1905,170 +1905,170 @@
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B66" t="s">
         <v>26</v>
       </c>
       <c r="C66" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E66" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B67" t="s">
         <v>26</v>
       </c>
       <c r="C67" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E67" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B68" t="s">
         <v>26</v>
       </c>
       <c r="C68" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E68" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B69" t="s">
         <v>24</v>
       </c>
       <c r="C69" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E69" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B70" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C70" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E70" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B71" t="s">
         <v>22</v>
       </c>
       <c r="C71" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E71" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B72" t="s">
+        <v>68</v>
+      </c>
+      <c r="C72" t="s">
         <v>69</v>
       </c>
-      <c r="C72" t="s">
-        <v>70</v>
-      </c>
       <c r="E72" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B73" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C73" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E73" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B74" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C74" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E74" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B77" t="s">
         <v>24</v>
       </c>
       <c r="C77" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E77" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B78" t="s">
         <v>24</v>
       </c>
       <c r="C78" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E78" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B79" t="s">
+        <v>74</v>
+      </c>
+      <c r="C79" t="s">
         <v>75</v>
       </c>
-      <c r="C79" t="s">
-        <v>76</v>
-      </c>
       <c r="E79" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
   </sheetData>

</xml_diff>